<commit_message>
another rule the world item
</commit_message>
<xml_diff>
--- a/rule-the-world/checklist.xlsx
+++ b/rule-the-world/checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/rule-the-world/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A3BFAAC-91DD-704C-BA4D-48F45F392FF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BFCA6C-C1AA-4641-A865-296AC1915E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="26740" windowHeight="15780" xr2:uid="{5DCC0A25-E991-BB4C-9021-D3E2E3BF72CA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>year</t>
   </si>
@@ -67,6 +67,21 @@
   </si>
   <si>
     <t>box set</t>
+  </si>
+  <si>
+    <t>wild7.jpg</t>
+  </si>
+  <si>
+    <t>Kokusai Tsushinsha</t>
+  </si>
+  <si>
+    <t>ワイルド7</t>
+  </si>
+  <si>
+    <t>Wild Seven</t>
+  </si>
+  <si>
+    <t>rulebook</t>
   </si>
 </sst>
 </file>
@@ -427,14 +442,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C14FC45-C471-4F4E-A96E-3BAD4D0CD00C}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
     <col min="5" max="5" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -478,6 +495,26 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2003</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>